<commit_message>
modified errors in the countries
</commit_message>
<xml_diff>
--- a/original_data/country.xlsx
+++ b/original_data/country.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seungyeonhan/Documents/GitHub/FinalExam_Visual/original_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7846142-BA46-B246-AB24-50DFEE8C256A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67906D57-26E4-7149-BA2E-8161BF8E6B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="24040" windowHeight="16000" xr2:uid="{78F09CA9-44AF-2243-908F-78B3C114ADBF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="574">
   <si>
     <t>Name</t>
   </si>
@@ -1755,6 +1755,9 @@
   </si>
   <si>
     <t>COD</t>
+  </si>
+  <si>
+    <t>The Democratic Republic of the Congo</t>
   </si>
 </sst>
 </file>
@@ -2122,10 +2125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D1EAFB1-A9CD-0C49-B612-1C17B69961CD}">
-  <dimension ref="A1:D329"/>
+  <dimension ref="A1:D330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
+      <selection activeCell="F322" sqref="F322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6643,7 +6646,7 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A323" s="2" t="s">
-        <v>554</v>
+        <v>573</v>
       </c>
       <c r="B323" t="s">
         <v>572</v>
@@ -6656,11 +6659,11 @@
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A324" s="1" t="s">
-        <v>564</v>
+      <c r="A324" s="2" t="s">
+        <v>554</v>
       </c>
       <c r="B324" t="s">
-        <v>117</v>
+        <v>572</v>
       </c>
       <c r="C324" t="s">
         <v>18</v>
@@ -6671,10 +6674,10 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A325" s="1" t="s">
-        <v>555</v>
+        <v>564</v>
       </c>
       <c r="B325" t="s">
-        <v>572</v>
+        <v>117</v>
       </c>
       <c r="C325" t="s">
         <v>18</v>
@@ -6685,7 +6688,7 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A326" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B326" t="s">
         <v>572</v>
@@ -6699,24 +6702,24 @@
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A327" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B327" t="s">
-        <v>558</v>
+        <v>572</v>
       </c>
       <c r="C327" t="s">
         <v>18</v>
       </c>
       <c r="D327" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A328" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B328" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C328" t="s">
         <v>18</v>
@@ -6726,7 +6729,21 @@
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A329" s="1"/>
+      <c r="A329" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="B329" t="s">
+        <v>560</v>
+      </c>
+      <c r="C329" t="s">
+        <v>18</v>
+      </c>
+      <c r="D329" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A330" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>